<commit_message>
updated and finished assignment 2 <3
</commit_message>
<xml_diff>
--- a/assignments/Excel Lab 2023 - Assignment 2 - conditional formatting, text manipulation and time.xlsx
+++ b/assignments/Excel Lab 2023 - Assignment 2 - conditional formatting, text manipulation and time.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anushkagupta/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Humna\Documents\GitHub\mis201\assignments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84707888-BDF2-5F46-B7C7-2AA575B87932}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32E08E2E-6719-4304-AFC2-3568CC6AD718}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="28800" windowHeight="16920" xr2:uid="{EC9BE8B5-70FB-4950-B36D-D16823981B32}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{EC9BE8B5-70FB-4950-B36D-D16823981B32}"/>
   </bookViews>
   <sheets>
     <sheet name="Conditional Formatting" sheetId="6" r:id="rId1"/>
@@ -612,7 +612,7 @@
     <numFmt numFmtId="164" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="h:mm:ss;@"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -986,7 +986,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1046,11 +1046,42 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="9">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -1156,12 +1187,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B42788A8-9DF4-4D2B-AAD0-989407AF7A66}" name="Table13" displayName="Table13" ref="A8:C28" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B42788A8-9DF4-4D2B-AAD0-989407AF7A66}" name="Table13" displayName="Table13" ref="A8:C28" totalsRowShown="0" headerRowDxfId="8" headerRowBorderDxfId="7" tableBorderDxfId="6">
   <autoFilter ref="A8:C28" xr:uid="{B42788A8-9DF4-4D2B-AAD0-989407AF7A66}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A9:C28">
+    <sortCondition descending="1" ref="C9:C28"/>
+  </sortState>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{A9EF1BAD-CAEA-4AEA-9A26-BFB75BB8C886}" name="Player" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{9A408912-4CE5-4A43-90D7-DBDA4585D0D7}" name="Mins Played " dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{D2CC32CF-3337-4DD1-AEAE-F940D4B3375D}" name="Goals Scored" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{A9EF1BAD-CAEA-4AEA-9A26-BFB75BB8C886}" name="Player" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{9A408912-4CE5-4A43-90D7-DBDA4585D0D7}" name="Mins Played " dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{D2CC32CF-3337-4DD1-AEAE-F940D4B3375D}" name="Goals Scored" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1464,37 +1498,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{982E556A-38C9-45A2-BA94-D5506BC869D6}">
-  <dimension ref="A1:N28"/>
+  <dimension ref="A1:N29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="93" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView topLeftCell="I20" zoomScale="93" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="25.5" customWidth="1"/>
-    <col min="2" max="3" width="15.83203125" customWidth="1"/>
-    <col min="6" max="6" width="25.5" customWidth="1"/>
-    <col min="7" max="8" width="15.83203125" customWidth="1"/>
-    <col min="11" max="11" width="25.5" customWidth="1"/>
-    <col min="12" max="13" width="15.83203125" customWidth="1"/>
+    <col min="1" max="1" width="25.453125" customWidth="1"/>
+    <col min="2" max="3" width="15.81640625" customWidth="1"/>
+    <col min="6" max="6" width="25.453125" customWidth="1"/>
+    <col min="7" max="8" width="15.81640625" customWidth="1"/>
+    <col min="11" max="11" width="25.453125" customWidth="1"/>
+    <col min="12" max="13" width="15.81640625" customWidth="1"/>
     <col min="14" max="14" width="37" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="23.5">
       <c r="A1" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" ht="23.5">
       <c r="A2" s="2"/>
     </row>
-    <row r="3" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="18.5">
       <c r="A3" s="4" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="24" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" ht="23.5">
       <c r="A4" s="3"/>
       <c r="B4" s="33">
         <v>10</v>
@@ -1506,7 +1540,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="86.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" ht="86.5" customHeight="1">
       <c r="A5" s="36" t="s">
         <v>91</v>
       </c>
@@ -1526,7 +1560,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14">
       <c r="A8" s="21" t="s">
         <v>64</v>
       </c>
@@ -1558,15 +1592,15 @@
         <v>87</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14">
       <c r="A9" s="19" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B9" s="5">
-        <v>2849</v>
+        <v>3271</v>
       </c>
       <c r="C9" s="20">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="F9" s="24" t="s">
         <v>67</v>
@@ -1586,16 +1620,20 @@
       <c r="M9" s="5">
         <v>13</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N9">
+        <f t="shared" ref="N9:N28" si="0">L9/M9</f>
+        <v>219.15384615384616</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
       <c r="A10" s="19" t="s">
-        <v>68</v>
+        <v>80</v>
       </c>
       <c r="B10" s="5">
-        <v>3445</v>
+        <v>3009</v>
       </c>
       <c r="C10" s="20">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="F10" s="24" t="s">
         <v>68</v>
@@ -1615,16 +1653,20 @@
       <c r="M10" s="5">
         <v>17</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N10">
+        <f t="shared" si="0"/>
+        <v>202.64705882352942</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
       <c r="A11" s="19" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="B11" s="5">
-        <v>2984</v>
+        <v>3392</v>
       </c>
       <c r="C11" s="20">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="F11" s="24" t="s">
         <v>69</v>
@@ -1644,16 +1686,20 @@
       <c r="M11" s="5">
         <v>13</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N11">
+        <f t="shared" si="0"/>
+        <v>229.53846153846155</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
       <c r="A12" s="19" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B12" s="5">
-        <v>3271</v>
+        <v>2836</v>
       </c>
       <c r="C12" s="20">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F12" s="24" t="s">
         <v>70</v>
@@ -1673,16 +1719,20 @@
       <c r="M12" s="5">
         <v>23</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N12">
+        <f t="shared" si="0"/>
+        <v>142.21739130434781</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
       <c r="A13" s="19" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="B13" s="5">
-        <v>2836</v>
+        <v>3045</v>
       </c>
       <c r="C13" s="20">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F13" s="24" t="s">
         <v>71</v>
@@ -1702,8 +1752,12 @@
       <c r="M13" s="5">
         <v>20</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N13">
+        <f t="shared" si="0"/>
+        <v>141.80000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
       <c r="A14" s="19" t="s">
         <v>72</v>
       </c>
@@ -1731,16 +1785,20 @@
       <c r="M14" s="5">
         <v>18</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N14">
+        <f t="shared" si="0"/>
+        <v>162.94444444444446</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
       <c r="A15" s="19" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="B15" s="5">
-        <v>2616</v>
+        <v>2801</v>
       </c>
       <c r="C15" s="20">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="F15" s="24" t="s">
         <v>73</v>
@@ -1760,13 +1818,17 @@
       <c r="M15" s="5">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N15">
+        <f t="shared" si="0"/>
+        <v>186.85714285714286</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
       <c r="A16" s="19" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B16" s="5">
-        <v>2788</v>
+        <v>3445</v>
       </c>
       <c r="C16" s="20">
         <v>17</v>
@@ -1789,16 +1851,20 @@
       <c r="M16" s="5">
         <v>17</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N16">
+        <f t="shared" si="0"/>
+        <v>164</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
       <c r="A17" s="19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B17" s="5">
-        <v>2130</v>
+        <v>2788</v>
       </c>
       <c r="C17" s="20">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="F17" s="24" t="s">
         <v>75</v>
@@ -1818,16 +1884,20 @@
       <c r="M17" s="5">
         <v>11</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N17">
+        <f t="shared" si="0"/>
+        <v>193.63636363636363</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
       <c r="A18" s="19" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B18" s="5">
-        <v>2663</v>
+        <v>2826</v>
       </c>
       <c r="C18" s="20">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="F18" s="24" t="s">
         <v>76</v>
@@ -1847,16 +1917,20 @@
       <c r="M18" s="5">
         <v>11</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N18">
+        <f t="shared" si="0"/>
+        <v>242.09090909090909</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14">
       <c r="A19" s="19" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="B19" s="5">
-        <v>2826</v>
+        <v>1566</v>
       </c>
       <c r="C19" s="20">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F19" s="24" t="s">
         <v>77</v>
@@ -1876,16 +1950,20 @@
       <c r="M19" s="5">
         <v>17</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N19">
+        <f t="shared" si="0"/>
+        <v>166.23529411764707</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
       <c r="A20" s="19" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="B20" s="5">
-        <v>3045</v>
+        <v>2380</v>
       </c>
       <c r="C20" s="20">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F20" s="24" t="s">
         <v>78</v>
@@ -1905,13 +1983,17 @@
       <c r="M20" s="5">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N20">
+        <f t="shared" si="0"/>
+        <v>160.26315789473685</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14">
       <c r="A21" s="19" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B21" s="5">
-        <v>2209</v>
+        <v>2616</v>
       </c>
       <c r="C21" s="20">
         <v>14</v>
@@ -1934,16 +2016,20 @@
       <c r="M21" s="5">
         <v>14</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N21">
+        <f t="shared" si="0"/>
+        <v>157.78571428571428</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14">
       <c r="A22" s="19" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B22" s="5">
-        <v>3009</v>
+        <v>2209</v>
       </c>
       <c r="C22" s="20">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="F22" s="24" t="s">
         <v>80</v>
@@ -1963,16 +2049,20 @@
       <c r="M22" s="5">
         <v>22</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N22">
+        <f t="shared" si="0"/>
+        <v>136.77272727272728</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14">
       <c r="A23" s="19" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="B23" s="5">
-        <v>3392</v>
+        <v>2849</v>
       </c>
       <c r="C23" s="20">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="F23" s="24" t="s">
         <v>81</v>
@@ -1992,16 +2082,20 @@
       <c r="M23" s="5">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N23">
+        <f t="shared" si="0"/>
+        <v>154.18181818181819</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14">
       <c r="A24" s="19" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="B24" s="5">
-        <v>2801</v>
+        <v>2984</v>
       </c>
       <c r="C24" s="20">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="F24" s="24" t="s">
         <v>82</v>
@@ -2021,8 +2115,12 @@
       <c r="M24" s="5">
         <v>18</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N24">
+        <f t="shared" si="0"/>
+        <v>155.61111111111111</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14">
       <c r="A25" s="19" t="s">
         <v>83</v>
       </c>
@@ -2050,13 +2148,17 @@
       <c r="M25" s="5">
         <v>13</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N25">
+        <f t="shared" si="0"/>
+        <v>253</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14">
       <c r="A26" s="19" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="B26" s="5">
-        <v>3087</v>
+        <v>2130</v>
       </c>
       <c r="C26" s="20">
         <v>11</v>
@@ -2079,16 +2181,20 @@
       <c r="M26" s="5">
         <v>11</v>
       </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N26">
+        <f t="shared" si="0"/>
+        <v>280.63636363636363</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14">
       <c r="A27" s="19" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="B27" s="5">
-        <v>2380</v>
+        <v>2663</v>
       </c>
       <c r="C27" s="20">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="F27" s="24" t="s">
         <v>85</v>
@@ -2108,16 +2214,20 @@
       <c r="M27" s="5">
         <v>15</v>
       </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N27">
+        <f t="shared" si="0"/>
+        <v>158.66666666666666</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14">
       <c r="A28" s="19" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B28" s="5">
-        <v>1566</v>
+        <v>3087</v>
       </c>
       <c r="C28" s="20">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="F28" s="26" t="s">
         <v>86</v>
@@ -2136,6 +2246,16 @@
       </c>
       <c r="M28" s="5">
         <v>16</v>
+      </c>
+      <c r="N28">
+        <f t="shared" si="0"/>
+        <v>97.875</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14">
+      <c r="H29">
+        <f>AVERAGE(H9:H28)</f>
+        <v>16.2</v>
       </c>
     </row>
   </sheetData>
@@ -2145,7 +2265,7 @@
     <mergeCell ref="K5:M5"/>
   </mergeCells>
   <conditionalFormatting sqref="B8">
-    <cfRule type="dataBar" priority="4">
+    <cfRule type="dataBar" priority="8">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2159,7 +2279,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G8">
-    <cfRule type="dataBar" priority="3">
+    <cfRule type="dataBar" priority="7">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2173,7 +2293,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L8">
-    <cfRule type="dataBar" priority="2">
+    <cfRule type="dataBar" priority="6">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2184,6 +2304,35 @@
           <x14:id>{F2C6C1CC-51E8-44C0-9EEF-CD7A0E193422}</x14:id>
         </ext>
       </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H9:H28">
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="greaterThan">
+      <formula>16.2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N9:N28">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K9:K28">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2242,31 +2391,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37ED1618-926B-4D36-8C2B-EDCA77F102B8}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView topLeftCell="A6" zoomScale="125" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" customWidth="1"/>
-    <col min="3" max="3" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" customWidth="1"/>
-    <col min="5" max="5" width="15.5" customWidth="1"/>
-    <col min="6" max="6" width="33.6640625" customWidth="1"/>
-    <col min="7" max="7" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="10.81640625" customWidth="1"/>
+    <col min="3" max="3" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.81640625" customWidth="1"/>
+    <col min="5" max="5" width="15.453125" customWidth="1"/>
+    <col min="6" max="6" width="33.6328125" customWidth="1"/>
+    <col min="7" max="7" width="28.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="23.5">
       <c r="A1" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="18.5">
       <c r="A3" s="4" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="24" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="23.5">
       <c r="A4" s="4"/>
       <c r="C4" s="33">
         <v>10</v>
@@ -2281,7 +2430,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="64" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="58">
       <c r="A5" s="4"/>
       <c r="C5" s="10" t="s">
         <v>57</v>
@@ -2296,7 +2445,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="58">
       <c r="A6" s="8" t="s">
         <v>0</v>
       </c>
@@ -2319,7 +2468,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -2342,185 +2491,329 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="6"/>
+      <c r="C8" s="6" t="str">
+        <f>LEFT(B8, 3)</f>
+        <v>Cha</v>
+      </c>
       <c r="D8" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E8" s="6" t="str">
+        <f>LEFT(D8, 3)</f>
+        <v>Rav</v>
+      </c>
+      <c r="F8" s="6" t="str">
+        <f>A8&amp;C8&amp;"_"&amp;E8&amp;"@hogwarts.edu"</f>
+        <v>ChoCha_Rav@hogwarts.edu</v>
+      </c>
+      <c r="G8" s="6" t="str">
+        <f>LOWER(F8)</f>
+        <v>chocha_rav@hogwarts.edu</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>9</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="6"/>
+      <c r="C9" s="6" t="str">
+        <f t="shared" ref="C9:C19" si="0">LEFT(B9, 3)</f>
+        <v>Mal</v>
+      </c>
       <c r="D9" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E9" s="6" t="str">
+        <f t="shared" ref="E9:E19" si="1">LEFT(D9, 3)</f>
+        <v>Sly</v>
+      </c>
+      <c r="F9" s="6" t="str">
+        <f t="shared" ref="F9:F19" si="2">A9&amp;C9&amp;"_"&amp;E9&amp;"@hogwarts.edu"</f>
+        <v>DracoMal_Sly@hogwarts.edu</v>
+      </c>
+      <c r="G9" s="6" t="str">
+        <f t="shared" ref="G9:G19" si="3">LOWER(F9)</f>
+        <v>dracomal_sly@hogwarts.edu</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
         <v>11</v>
       </c>
       <c r="B10" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="6"/>
+      <c r="C10" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Mac</v>
+      </c>
       <c r="D10" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E10" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>Huf</v>
+      </c>
+      <c r="F10" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>ErnieMac_Huf@hogwarts.edu</v>
+      </c>
+      <c r="G10" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>erniemac_huf@hogwarts.edu</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>14</v>
       </c>
       <c r="B11" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="6"/>
+      <c r="C11" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Pot</v>
+      </c>
       <c r="D11" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E11" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>Gry</v>
+      </c>
+      <c r="F11" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>HarryPot_Gry@hogwarts.edu</v>
+      </c>
+      <c r="G11" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>harrypot_gry@hogwarts.edu</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
         <v>17</v>
       </c>
       <c r="B12" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="6"/>
+      <c r="C12" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Gra</v>
+      </c>
       <c r="D12" t="s">
         <v>16</v>
       </c>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E12" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>Gry</v>
+      </c>
+      <c r="F12" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>HermioneGra_Gry@hogwarts.edu</v>
+      </c>
+      <c r="G12" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>hermionegra_gry@hogwarts.edu</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" t="s">
         <v>19</v>
       </c>
       <c r="B13" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="6"/>
+      <c r="C13" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Fin</v>
+      </c>
       <c r="D13" t="s">
         <v>13</v>
       </c>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E13" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>Huf</v>
+      </c>
+      <c r="F13" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>JustinFin_Huf@hogwarts.edu</v>
+      </c>
+      <c r="G13" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>justinfin_huf@hogwarts.edu</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" t="s">
         <v>21</v>
       </c>
       <c r="B14" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="6"/>
+      <c r="C14" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Lov</v>
+      </c>
       <c r="D14" t="s">
         <v>8</v>
       </c>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E14" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>Rav</v>
+      </c>
+      <c r="F14" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>LunaLov_Rav@hogwarts.edu</v>
+      </c>
+      <c r="G14" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>lunalov_rav@hogwarts.edu</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15" t="s">
         <v>23</v>
       </c>
       <c r="B15" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="6"/>
+      <c r="C15" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Lon</v>
+      </c>
       <c r="D15" t="s">
         <v>16</v>
       </c>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E15" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>Gry</v>
+      </c>
+      <c r="F15" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>NevilleLon_Gry@hogwarts.edu</v>
+      </c>
+      <c r="G15" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>nevillelon_gry@hogwarts.edu</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16" t="s">
         <v>25</v>
       </c>
       <c r="B16" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="6"/>
+      <c r="C16" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Pat</v>
+      </c>
       <c r="D16" t="s">
         <v>8</v>
       </c>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E16" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>Rav</v>
+      </c>
+      <c r="F16" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>PadmaPat_Rav@hogwarts.edu</v>
+      </c>
+      <c r="G16" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>padmapat_rav@hogwarts.edu</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" t="s">
         <v>27</v>
       </c>
       <c r="B17" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="6"/>
+      <c r="C17" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Par</v>
+      </c>
       <c r="D17" t="s">
         <v>5</v>
       </c>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E17" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>Sly</v>
+      </c>
+      <c r="F17" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>PansyPar_Sly@hogwarts.edu</v>
+      </c>
+      <c r="G17" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>pansypar_sly@hogwarts.edu</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18" t="s">
         <v>29</v>
       </c>
       <c r="B18" t="s">
         <v>30</v>
       </c>
-      <c r="C18" s="6"/>
+      <c r="C18" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Wea</v>
+      </c>
       <c r="D18" t="s">
         <v>16</v>
       </c>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E18" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>Gry</v>
+      </c>
+      <c r="F18" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>RonWea_Gry@hogwarts.edu</v>
+      </c>
+      <c r="G18" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>ronwea_gry@hogwarts.edu</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19" t="s">
         <v>31</v>
       </c>
       <c r="B19" t="s">
         <v>32</v>
       </c>
-      <c r="C19" s="6"/>
+      <c r="C19" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Bon</v>
+      </c>
       <c r="D19" t="s">
         <v>13</v>
       </c>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
+      <c r="E19" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>Huf</v>
+      </c>
+      <c r="F19" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>SusanBon_Huf@hogwarts.edu</v>
+      </c>
+      <c r="G19" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>susanbon_huf@hogwarts.edu</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2531,34 +2824,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E705A9A-7B7C-4B21-B7A9-C21F1D64D294}">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView zoomScale="141" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="141" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="17.5" customWidth="1"/>
-    <col min="2" max="2" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1640625" customWidth="1"/>
-    <col min="5" max="5" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.33203125" customWidth="1"/>
+    <col min="1" max="1" width="17.453125" customWidth="1"/>
+    <col min="2" max="2" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" customWidth="1"/>
+    <col min="5" max="5" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.6328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="23.5">
       <c r="A1" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="23.5">
       <c r="A2" s="2"/>
     </row>
-    <row r="3" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="18.5">
       <c r="A3" s="4" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="24" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="23.5">
       <c r="E4" s="33">
         <v>5</v>
       </c>
@@ -2569,7 +2862,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="87">
       <c r="C5" s="1"/>
       <c r="E5" s="10" t="s">
         <v>60</v>
@@ -2581,7 +2874,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8">
       <c r="A6" s="11" t="s">
         <v>37</v>
       </c>
@@ -2604,7 +2897,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" ht="15.5">
       <c r="A7" s="12" t="s">
         <v>43</v>
       </c>
@@ -2617,11 +2910,20 @@
       <c r="D7" s="14">
         <v>0.70833333333333337</v>
       </c>
-      <c r="E7" s="16"/>
-      <c r="F7" s="32"/>
-      <c r="G7" s="17"/>
-    </row>
-    <row r="8" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="E7" s="16">
+        <f>(D7-C7)</f>
+        <v>0.37500000000000006</v>
+      </c>
+      <c r="F7" s="32">
+        <f>E7*24</f>
+        <v>9.0000000000000018</v>
+      </c>
+      <c r="G7" s="17">
+        <f>F7*B7</f>
+        <v>900.00000000000023</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15.5">
       <c r="A8" s="12" t="s">
         <v>44</v>
       </c>
@@ -2634,11 +2936,20 @@
       <c r="D8" s="14">
         <v>0.66666666666666663</v>
       </c>
-      <c r="E8" s="16"/>
-      <c r="F8" s="32"/>
-      <c r="G8" s="17"/>
-    </row>
-    <row r="9" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="E8" s="16">
+        <f t="shared" ref="E8:E11" si="0">(D8-C8)</f>
+        <v>0.27083333333333331</v>
+      </c>
+      <c r="F8" s="32">
+        <f t="shared" ref="F8:F11" si="1">E8*24</f>
+        <v>6.5</v>
+      </c>
+      <c r="G8" s="17">
+        <f>F8*B8</f>
+        <v>650</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15.5">
       <c r="A9" s="12" t="s">
         <v>45</v>
       </c>
@@ -2651,11 +2962,20 @@
       <c r="D9" s="14">
         <v>0.75</v>
       </c>
-      <c r="E9" s="16"/>
-      <c r="F9" s="32"/>
-      <c r="G9" s="17"/>
-    </row>
-    <row r="10" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="E9" s="16">
+        <f t="shared" si="0"/>
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="F9" s="32">
+        <f t="shared" si="1"/>
+        <v>8.5</v>
+      </c>
+      <c r="G9" s="17">
+        <f>F9*B9</f>
+        <v>850</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15.5">
       <c r="A10" s="12" t="s">
         <v>46</v>
       </c>
@@ -2668,11 +2988,20 @@
       <c r="D10" s="14">
         <v>0.70833333333333337</v>
       </c>
-      <c r="E10" s="16"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="17"/>
-    </row>
-    <row r="11" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="E10" s="16">
+        <f t="shared" si="0"/>
+        <v>0.31250000000000006</v>
+      </c>
+      <c r="F10" s="32">
+        <f t="shared" si="1"/>
+        <v>7.5000000000000018</v>
+      </c>
+      <c r="G10" s="17">
+        <f t="shared" ref="G8:G11" si="2">F10*B10</f>
+        <v>600.00000000000011</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15.5">
       <c r="A11" s="12" t="s">
         <v>47</v>
       </c>
@@ -2685,15 +3014,27 @@
       <c r="D11" s="14">
         <v>0.70833333333333337</v>
       </c>
-      <c r="E11" s="16"/>
-      <c r="F11" s="32"/>
-      <c r="G11" s="17"/>
-    </row>
-    <row r="13" spans="1:8" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E11" s="16">
+        <f t="shared" si="0"/>
+        <v>0.31250000000000006</v>
+      </c>
+      <c r="F11" s="32">
+        <f t="shared" si="1"/>
+        <v>7.5000000000000018</v>
+      </c>
+      <c r="G11" s="17">
+        <f t="shared" si="2"/>
+        <v>600.00000000000011</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="27.5" customHeight="1">
       <c r="F13" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="G13" s="17"/>
+      <c r="G13" s="37">
+        <f>SUM(G7:G11)</f>
+        <v>3600</v>
+      </c>
       <c r="H13" s="33">
         <v>5</v>
       </c>

</xml_diff>